<commit_message>
Ajout data partie 1
</commit_message>
<xml_diff>
--- a/data_csv/Equipement.xlsx
+++ b/data_csv/Equipement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\MaisonEconome\data_csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA16F5B6-D765-4225-BCBA-EE86D856A90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F989FEE-83D7-4C39-A115-EB9ABBB7C45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2220" yWindow="2880" windowWidth="17280" windowHeight="8964" xr2:uid="{35907681-4874-480C-8734-055EFBFFF0E4}"/>
   </bookViews>
@@ -402,13 +402,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCE748F5-6D50-41E9-BA91-AE1FF609F77A}">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -552,6 +559,381 @@
         <v>25</v>
       </c>
     </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
ajout data partie 2
</commit_message>
<xml_diff>
--- a/data_csv/Equipement.xlsx
+++ b/data_csv/Equipement.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\wamp64\www\MaisonEconome\data_csv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F989FEE-83D7-4C39-A115-EB9ABBB7C45E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9523866-596E-4379-BE03-DAE411EB2FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2220" yWindow="2880" windowWidth="17280" windowHeight="8964" xr2:uid="{35907681-4874-480C-8734-055EFBFFF0E4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{35907681-4874-480C-8734-055EFBFFF0E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="16">
   <si>
     <t>equipementId</t>
   </si>
@@ -51,6 +51,39 @@
   </si>
   <si>
     <t>typeEquipementId</t>
+  </si>
+  <si>
+    <t>grille pain</t>
+  </si>
+  <si>
+    <t>micro-onde</t>
+  </si>
+  <si>
+    <t>fer à repasser</t>
+  </si>
+  <si>
+    <t>réfrigirateur</t>
+  </si>
+  <si>
+    <t>four</t>
+  </si>
+  <si>
+    <t>machine à laver</t>
+  </si>
+  <si>
+    <t>ordinateur</t>
+  </si>
+  <si>
+    <t>console de jeux</t>
+  </si>
+  <si>
+    <t>télévision</t>
+  </si>
+  <si>
+    <t>cheminée</t>
+  </si>
+  <si>
+    <t>gazinière</t>
   </si>
 </sst>
 </file>
@@ -86,8 +119,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,14 +439,14 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.77734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -438,500 +472,1550 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2" t="str">
+        <f ca="1">_xlfn.CONCAT("lampe n°", RANDBETWEEN(1,3))</f>
+        <v>lampe n°3</v>
+      </c>
+      <c r="C2" t="str">
+        <f ca="1">IF(RANDBETWEEN(0,1)=0,"Despcription brève de l'équipement", "")</f>
+        <v/>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" t="str">
+        <f t="shared" ref="B3:B21" ca="1" si="0">_xlfn.CONCAT("lampe n°", RANDBETWEEN(1,3))</f>
+        <v>lampe n°2</v>
+      </c>
+      <c r="C3" t="str">
+        <f t="shared" ref="C3:C66" ca="1" si="1">IF(RANDBETWEEN(0,1)=0,"Despcription brève de l'équipement", "")</f>
+        <v/>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
+      </c>
+      <c r="B4" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°3</v>
+      </c>
+      <c r="C4" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
+      <c r="B5" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°1</v>
+      </c>
+      <c r="C5" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°1</v>
+      </c>
+      <c r="C6" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
+      <c r="B7" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°3</v>
+      </c>
+      <c r="C7" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
+      <c r="B8" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°1</v>
+      </c>
+      <c r="C8" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
+      <c r="B9" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°3</v>
+      </c>
+      <c r="C9" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
+      <c r="B10" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°2</v>
+      </c>
+      <c r="C10" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
+      <c r="B11" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°2</v>
+      </c>
+      <c r="C11" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
+      <c r="B12" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°3</v>
+      </c>
+      <c r="C12" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
+      <c r="B13" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°2</v>
+      </c>
+      <c r="C13" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
+      <c r="B14" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°3</v>
+      </c>
+      <c r="C14" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
+      <c r="B15" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°1</v>
+      </c>
+      <c r="C15" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°1</v>
+      </c>
+      <c r="C16" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°1</v>
+      </c>
+      <c r="C17" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°2</v>
+      </c>
+      <c r="C18" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°3</v>
+      </c>
+      <c r="C19" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°3</v>
+      </c>
+      <c r="C20" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="str">
+        <f t="shared" ca="1" si="0"/>
+        <v>lampe n°3</v>
+      </c>
+      <c r="C21" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="str">
+        <f>_xlfn.CONCAT("lampe de chevet")</f>
+        <v>lampe de chevet</v>
+      </c>
+      <c r="C22" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="str">
+        <f t="shared" ref="B23:B32" si="2">_xlfn.CONCAT("lampe de chevet")</f>
+        <v>lampe de chevet</v>
+      </c>
+      <c r="C23" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>lampe de chevet</v>
+      </c>
+      <c r="C24" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>lampe de chevet</v>
+      </c>
+      <c r="C25" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>lampe de chevet</v>
+      </c>
+      <c r="C26" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>lampe de chevet</v>
+      </c>
+      <c r="C27" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>lampe de chevet</v>
+      </c>
+      <c r="C28" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>lampe de chevet</v>
+      </c>
+      <c r="C29" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>lampe de chevet</v>
+      </c>
+      <c r="C30" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="str">
+        <f t="shared" si="2"/>
+        <v>lampe de chevet</v>
+      </c>
+      <c r="C31" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="str">
+        <f t="shared" ref="B32:B36" si="3">_xlfn.CONCAT("lampe fantaisie")</f>
+        <v>lampe fantaisie</v>
+      </c>
+      <c r="C32" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>lampe fantaisie</v>
+      </c>
+      <c r="C33" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" s="1" t="str">
+        <f>_xlfn.CONCAT("lampe fantaisie")</f>
+        <v>lampe fantaisie</v>
+      </c>
+      <c r="C34" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>lampe fantaisie</v>
+      </c>
+      <c r="C35" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="str">
+        <f t="shared" si="3"/>
+        <v>lampe fantaisie</v>
+      </c>
+      <c r="C36" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" t="str">
+        <f ca="1">_xlfn.CONCAT("spot n°", RANDBETWEEN(1,3))</f>
+        <v>spot n°3</v>
+      </c>
+      <c r="C37" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" t="str">
+        <f t="shared" ref="B38:B41" ca="1" si="4">_xlfn.CONCAT("spot n°", RANDBETWEEN(1,3))</f>
+        <v>spot n°3</v>
+      </c>
+      <c r="C38" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>spot n°1</v>
+      </c>
+      <c r="C39" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>spot n°2</v>
+      </c>
+      <c r="C40" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" t="str">
+        <f t="shared" ca="1" si="4"/>
+        <v>spot n°3</v>
+      </c>
+      <c r="C41" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>5</v>
+      </c>
+      <c r="C42" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>5</v>
+      </c>
+      <c r="C43" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E43">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>5</v>
+      </c>
+      <c r="C44" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>5</v>
+      </c>
+      <c r="C45" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E45">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>5</v>
+      </c>
+      <c r="C46" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>6</v>
+      </c>
+      <c r="C47" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>6</v>
+      </c>
+      <c r="C48" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E48">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>6</v>
+      </c>
+      <c r="C49" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E49">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E50">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>6</v>
+      </c>
+      <c r="C51" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>7</v>
+      </c>
+      <c r="C52" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>7</v>
+      </c>
+      <c r="C53" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E53">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>7</v>
+      </c>
+      <c r="C54" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>7</v>
+      </c>
+      <c r="C55" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E55">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>7</v>
+      </c>
+      <c r="C56" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
+        <v>8</v>
+      </c>
+      <c r="C58" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E58">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B59" t="s">
+        <v>8</v>
+      </c>
+      <c r="C59" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E59">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B60" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B61" t="s">
+        <v>8</v>
+      </c>
+      <c r="C61" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E61">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B63" t="s">
+        <v>9</v>
+      </c>
+      <c r="C63" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E63">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E65">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B66" t="s">
+        <v>9</v>
+      </c>
+      <c r="C66" t="str">
+        <f t="shared" ca="1" si="1"/>
+        <v/>
+      </c>
+      <c r="E66">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B67" t="s">
+        <v>15</v>
+      </c>
+      <c r="C67" t="str">
+        <f t="shared" ref="C67:C101" ca="1" si="5">IF(RANDBETWEEN(0,1)=0,"Despcription brève de l'équipement", "")</f>
+        <v/>
+      </c>
+      <c r="E67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B68" t="s">
+        <v>15</v>
+      </c>
+      <c r="C68" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E68">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B69" t="s">
+        <v>15</v>
+      </c>
+      <c r="C69" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B70" t="s">
+        <v>15</v>
+      </c>
+      <c r="C70" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E70">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A71">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B71" t="s">
+        <v>15</v>
+      </c>
+      <c r="C71" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E71">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B72" t="s">
+        <v>15</v>
+      </c>
+      <c r="C72" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E72">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A73">
         <v>72</v>
       </c>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B73" t="s">
+        <v>15</v>
+      </c>
+      <c r="C73" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B74" t="s">
+        <v>15</v>
+      </c>
+      <c r="C74" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E74">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B75" t="s">
+        <v>15</v>
+      </c>
+      <c r="C75" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E75">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B76" t="s">
+        <v>15</v>
+      </c>
+      <c r="C76" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E76">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B77" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E77">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B78" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E78">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B79" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E79">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A80">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B80" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E80">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B81" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B82" t="s">
+        <v>13</v>
+      </c>
+      <c r="C82" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E82">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B83" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E83">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B84" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B85" t="s">
+        <v>12</v>
+      </c>
+      <c r="C85" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E85">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B86" t="s">
+        <v>12</v>
+      </c>
+      <c r="C86" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E86">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B87" t="s">
+        <v>14</v>
+      </c>
+      <c r="C87" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E87">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B88" t="s">
+        <v>14</v>
+      </c>
+      <c r="C88" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E88">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B89" t="s">
+        <v>14</v>
+      </c>
+      <c r="C89" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E89">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B90" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E90">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B91" t="s">
+        <v>14</v>
+      </c>
+      <c r="C91" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E91">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B92" t="str">
+        <f ca="1">_xlfn.CONCAT("radiateur n°", RANDBETWEEN(1,3))</f>
+        <v>radiateur n°3</v>
+      </c>
+      <c r="C92" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E92">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B93" t="str">
+        <f t="shared" ref="B93:B101" ca="1" si="6">_xlfn.CONCAT("radiateur n°", RANDBETWEEN(1,3))</f>
+        <v>radiateur n°1</v>
+      </c>
+      <c r="C93" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E93">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B94" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>radiateur n°2</v>
+      </c>
+      <c r="C94" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E94">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B95" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>radiateur n°3</v>
+      </c>
+      <c r="C95" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E95">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B96" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>radiateur n°2</v>
+      </c>
+      <c r="C96" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E96">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B97" t="str">
+        <f ca="1">_xlfn.CONCAT("radiateur n°", RANDBETWEEN(1,3))</f>
+        <v>radiateur n°1</v>
+      </c>
+      <c r="C97" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E97">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B98" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>radiateur n°1</v>
+      </c>
+      <c r="C98" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E98">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B99" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>radiateur n°1</v>
+      </c>
+      <c r="C99" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B100" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>radiateur n°2</v>
+      </c>
+      <c r="C100" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v/>
+      </c>
+      <c r="E100">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A101">
         <v>100</v>
+      </c>
+      <c r="B101" t="str">
+        <f t="shared" ca="1" si="6"/>
+        <v>radiateur n°2</v>
+      </c>
+      <c r="C101" t="str">
+        <f t="shared" ca="1" si="5"/>
+        <v>Despcription brève de l'équipement</v>
+      </c>
+      <c r="E101">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>